<commit_message>
last update to lambda.xlsx
</commit_message>
<xml_diff>
--- a/report/lambda.xlsx
+++ b/report/lambda.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="0" windowWidth="15840" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2720" yWindow="0" windowWidth="19900" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Lambda</t>
   </si>
@@ -34,6 +34,30 @@
   </si>
   <si>
     <t>Accuracy training</t>
+  </si>
+  <si>
+    <t>Training - Test</t>
+  </si>
+  <si>
+    <t>Validation - Test</t>
+  </si>
+  <si>
+    <t>Average validation accuracy</t>
+  </si>
+  <si>
+    <t>Average training accuracy</t>
+  </si>
+  <si>
+    <t>Average test accuracy</t>
+  </si>
+  <si>
+    <t>Max training accuracy</t>
+  </si>
+  <si>
+    <t>Max validation accuracy</t>
+  </si>
+  <si>
+    <t>Max test accuracy</t>
   </si>
 </sst>
 </file>
@@ -90,8 +114,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -124,7 +198,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -137,6 +211,31 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -149,6 +248,31 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -490,9 +614,17 @@
     <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="19.5" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.83203125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -508,8 +640,32 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>4</v>
       </c>
@@ -525,8 +681,40 @@
       <c r="E2" s="2">
         <v>0.70609999999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="2">
+        <f>C2-E2</f>
+        <v>6.0800000000000853E-3</v>
+      </c>
+      <c r="G2" s="2">
+        <f>D2-E2</f>
+        <v>1.3000000000000012E-2</v>
+      </c>
+      <c r="H2" s="2">
+        <f>AVERAGE(C2:C12)</f>
+        <v>0.74023818181818168</v>
+      </c>
+      <c r="I2" s="2">
+        <f>AVERAGE(D2:D12)</f>
+        <v>0.7353909090909091</v>
+      </c>
+      <c r="J2" s="2">
+        <f>AVERAGE(E2:E12)</f>
+        <v>0.73757272727272738</v>
+      </c>
+      <c r="K2" s="2">
+        <f>MAX(C2:C12)</f>
+        <v>0.85824</v>
+      </c>
+      <c r="L2" s="2">
+        <f>MAX(D2:D12)</f>
+        <v>0.84909999999999997</v>
+      </c>
+      <c r="M2" s="2">
+        <f>MAX(E2:E12)</f>
+        <v>0.85250000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <v>4</v>
       </c>
@@ -542,8 +730,16 @@
       <c r="E3" s="2">
         <v>0.85250000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F56" si="0">C3-E3</f>
+        <v>5.7399999999999674E-3</v>
+      </c>
+      <c r="G3" s="2">
+        <f t="shared" ref="G3:G56" si="1">D3-E3</f>
+        <v>-3.4000000000000696E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
         <v>4</v>
       </c>
@@ -559,8 +755,16 @@
       <c r="E4" s="2">
         <v>0.83430000000000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.6000000000000467E-3</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.9000000000000146E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
         <v>4</v>
       </c>
@@ -576,8 +780,16 @@
       <c r="E5" s="2">
         <v>0.79300000000000004</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>3.3799999999999386E-3</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.8000000000000282E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
         <v>4</v>
       </c>
@@ -593,8 +805,16 @@
       <c r="E6" s="2">
         <v>0.79590000000000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>4.4599999999999085E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9999999999992291E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>4</v>
       </c>
@@ -610,8 +830,16 @@
       <c r="E7" s="2">
         <v>0.61470000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>8.579999999999921E-3</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>9.000000000000119E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>4</v>
       </c>
@@ -627,8 +855,16 @@
       <c r="E8" s="2">
         <v>0.77100000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6599999999999975E-3</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999908E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>4</v>
       </c>
@@ -644,8 +880,16 @@
       <c r="E9" s="2">
         <v>0.72650000000000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5399999999999894E-3</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.8000000000000282E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>4</v>
       </c>
@@ -661,8 +905,16 @@
       <c r="E10" s="2">
         <v>0.82169999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000238E-3</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.1999999999999815E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>4</v>
       </c>
@@ -678,8 +930,16 @@
       <c r="E11" s="2">
         <v>0.43990000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.8199999999999918E-3</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.040000000000002E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>4</v>
       </c>
@@ -695,8 +955,16 @@
       <c r="E12" s="2">
         <v>0.75770000000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.5000000000000577E-3</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.2000000000000934E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>8</v>
       </c>
@@ -712,8 +980,40 @@
       <c r="E13" s="2">
         <v>0.89500000000000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>7.4600000000000222E-3</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.1999999999999789E-3</v>
+      </c>
+      <c r="H13" s="2">
+        <f>AVERAGE(C13:C23)</f>
+        <v>0.91371090909090924</v>
+      </c>
+      <c r="I13" s="2">
+        <f>AVERAGE(D13:D23)</f>
+        <v>0.90366363636363645</v>
+      </c>
+      <c r="J13" s="2">
+        <f>AVERAGE(E13:E23)</f>
+        <v>0.90742727272727253</v>
+      </c>
+      <c r="K13" s="2">
+        <f>MAX(C13:C23)</f>
+        <v>0.92779999999999996</v>
+      </c>
+      <c r="L13" s="2">
+        <f>MAX(D13:D23)</f>
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="M13" s="2">
+        <f>MAX(E13:E23)</f>
+        <v>0.91879999999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>8</v>
       </c>
@@ -729,8 +1029,16 @@
       <c r="E14" s="2">
         <v>0.91779999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="2">
+        <f t="shared" si="0"/>
+        <v>6.5800000000000303E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.0799999999999921E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>8</v>
       </c>
@@ -746,8 +1054,16 @@
       <c r="E15" s="2">
         <v>0.90580000000000005</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="2">
+        <f t="shared" si="0"/>
+        <v>7.7599999999999891E-3</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5999999999999348E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16">
         <v>8</v>
       </c>
@@ -763,8 +1079,16 @@
       <c r="E16" s="2">
         <v>0.90239999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="2">
+        <f t="shared" si="0"/>
+        <v>5.2200000000000024E-3</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.0000000000000062E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17">
         <v>8</v>
       </c>
@@ -780,8 +1104,16 @@
       <c r="E17" s="2">
         <v>0.91420000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="2">
+        <f t="shared" si="0"/>
+        <v>6.0399999999999343E-3</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.8000000000000291E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18">
         <v>8</v>
       </c>
@@ -797,8 +1129,16 @@
       <c r="E18" s="2">
         <v>0.90169999999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3000000000000789E-3</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.9999999999998952E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19">
         <v>8</v>
       </c>
@@ -814,8 +1154,16 @@
       <c r="E19" s="2">
         <v>0.91090000000000004</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="2">
+        <f t="shared" si="0"/>
+        <v>9.4599999999999129E-3</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20">
         <v>8</v>
       </c>
@@ -831,8 +1179,16 @@
       <c r="E20" s="2">
         <v>0.91879999999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="2">
+        <f t="shared" si="0"/>
+        <v>9.000000000000008E-3</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.2999999999999696E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21">
         <v>8</v>
       </c>
@@ -848,8 +1204,16 @@
       <c r="E21" s="2">
         <v>0.90849999999999997</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9799999999999871E-3</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.3999999999999586E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22">
         <v>8</v>
       </c>
@@ -865,8 +1229,16 @@
       <c r="E22" s="2">
         <v>0.90580000000000005</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="2">
+        <f t="shared" si="0"/>
+        <v>2.7399999999999647E-3</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.9000000000000181E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23">
         <v>8</v>
       </c>
@@ -882,8 +1254,16 @@
       <c r="E23" s="2">
         <v>0.90080000000000005</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
+        <v>5.5799999999999184E-3</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24">
         <v>12</v>
       </c>
@@ -899,8 +1279,40 @@
       <c r="E24" s="2">
         <v>0.92559999999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="2">
+        <f t="shared" si="0"/>
+        <v>8.720000000000061E-3</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.6999999999999238E-3</v>
+      </c>
+      <c r="H24" s="2">
+        <f>AVERAGE(C24:C34)</f>
+        <v>0.93885454545454516</v>
+      </c>
+      <c r="I24" s="2">
+        <f>AVERAGE(D24:D34)</f>
+        <v>0.92418181818181822</v>
+      </c>
+      <c r="J24" s="2">
+        <f>AVERAGE(E24:E34)</f>
+        <v>0.92838181818181831</v>
+      </c>
+      <c r="K24" s="2">
+        <f>MAX(C24:C34)</f>
+        <v>0.94743999999999995</v>
+      </c>
+      <c r="L24" s="2">
+        <f>MAX(D24:D34)</f>
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="M24" s="2">
+        <f>MAX(E24:E34)</f>
+        <v>0.93620000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25">
         <v>12</v>
       </c>
@@ -916,8 +1328,16 @@
       <c r="E25" s="2">
         <v>0.93220000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="2">
+        <f t="shared" si="0"/>
+        <v>1.523999999999992E-2</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26">
         <v>12</v>
       </c>
@@ -933,8 +1353,16 @@
       <c r="E26" s="2">
         <v>0.9244</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4059999999999961E-2</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.0999999999999908E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27">
         <v>12</v>
       </c>
@@ -950,8 +1378,16 @@
       <c r="E27" s="2">
         <v>0.92820000000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9799999999999889E-3</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.0999999999999961E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28">
         <v>12</v>
       </c>
@@ -967,8 +1403,16 @@
       <c r="E28" s="2">
         <v>0.93620000000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>9.2399999999999149E-3</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.0999999999999943E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29">
         <v>12</v>
       </c>
@@ -984,8 +1428,16 @@
       <c r="E29" s="2">
         <v>0.92800000000000005</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1159999999999948E-2</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.6000000000000485E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30">
         <v>12</v>
       </c>
@@ -1001,8 +1453,16 @@
       <c r="E30" s="2">
         <v>0.92379999999999995</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="2">
+        <f t="shared" si="0"/>
+        <v>7.6000000000000512E-3</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.7999999999999146E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31">
         <v>12</v>
       </c>
@@ -1018,8 +1478,16 @@
       <c r="E31" s="2">
         <v>0.93020000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0799999999999921E-2</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.2999999999999732E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32">
         <v>12</v>
       </c>
@@ -1035,8 +1503,16 @@
       <c r="E32" s="2">
         <v>0.93020000000000003</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="2">
+        <f t="shared" si="0"/>
+        <v>1.205999999999996E-2</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.4000000000000687E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33">
         <v>12</v>
       </c>
@@ -1052,8 +1528,16 @@
       <c r="E33" s="2">
         <v>0.92800000000000005</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2899999999999912E-2</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>-9.000000000000119E-4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34">
         <v>12</v>
       </c>
@@ -1069,8 +1553,16 @@
       <c r="E34" s="2">
         <v>0.9254</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4399999999999986E-3</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.1999999999999833E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35">
         <v>16</v>
       </c>
@@ -1086,8 +1578,40 @@
       <c r="E35" s="2">
         <v>0.94299999999999995</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9400000000000581E-3</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.5999999999999366E-3</v>
+      </c>
+      <c r="H35" s="2">
+        <f>AVERAGE(C35:C45)</f>
+        <v>0.95205999999999991</v>
+      </c>
+      <c r="I35" s="2">
+        <f>AVERAGE(D35:D45)</f>
+        <v>0.93747272727272746</v>
+      </c>
+      <c r="J35" s="2">
+        <f>AVERAGE(E35:E45)</f>
+        <v>0.94045454545454554</v>
+      </c>
+      <c r="K35" s="2">
+        <f>MAX(C35:C45)</f>
+        <v>0.95720000000000005</v>
+      </c>
+      <c r="L35" s="2">
+        <f>MAX(D35:D45)</f>
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="M35" s="2">
+        <f>MAX(E35:E45)</f>
+        <v>0.94450000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36">
         <v>16</v>
       </c>
@@ -1103,8 +1627,16 @@
       <c r="E36" s="2">
         <v>0.93810000000000004</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4440000000000008E-2</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37">
         <v>16</v>
       </c>
@@ -1120,8 +1652,16 @@
       <c r="E37" s="2">
         <v>0.9385</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="2">
+        <f t="shared" si="0"/>
+        <v>9.8799999999999999E-3</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>-4.4999999999999485E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38">
         <v>16</v>
       </c>
@@ -1137,8 +1677,16 @@
       <c r="E38" s="2">
         <v>0.94030000000000002</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1639999999999984E-2</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.4000000000000696E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39">
         <v>16</v>
       </c>
@@ -1154,8 +1702,16 @@
       <c r="E39" s="2">
         <v>0.93820000000000003</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="2">
+        <f t="shared" si="0"/>
+        <v>1.100000000000001E-2</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="1"/>
+        <v>-2.4000000000000687E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40">
         <v>16</v>
       </c>
@@ -1171,8 +1727,16 @@
       <c r="E40" s="2">
         <v>0.94450000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2700000000000045E-2</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.3999999999999586E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41">
         <v>16</v>
       </c>
@@ -1188,8 +1752,16 @@
       <c r="E41" s="2">
         <v>0.9355</v>
       </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5639999999999987E-2</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.9999999999995595E-4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42">
         <v>16</v>
       </c>
@@ -1205,8 +1777,16 @@
       <c r="E42" s="2">
         <v>0.94120000000000004</v>
       </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="2">
+        <f t="shared" si="0"/>
+        <v>1.091999999999993E-2</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.3000000000000789E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43">
         <v>16</v>
       </c>
@@ -1222,8 +1802,16 @@
       <c r="E43" s="2">
         <v>0.94369999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0380000000000056E-2</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.3999999999999613E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44">
         <v>16</v>
       </c>
@@ -1239,8 +1827,16 @@
       <c r="E44" s="2">
         <v>0.94079999999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4380000000000059E-2</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.9999999999993392E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45">
         <v>16</v>
       </c>
@@ -1256,8 +1852,16 @@
       <c r="E45" s="2">
         <v>0.94120000000000004</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="2">
+        <f t="shared" si="0"/>
+        <v>8.73999999999997E-3</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="1"/>
+        <v>-9.8000000000000309E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46">
         <v>20</v>
       </c>
@@ -1273,8 +1877,40 @@
       <c r="E46" s="2">
         <v>0.94750000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1259999999999937E-2</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="1"/>
+        <v>-7.5000000000000622E-3</v>
+      </c>
+      <c r="H46" s="2">
+        <f>AVERAGE(C46:C56)</f>
+        <v>0.95550363636363622</v>
+      </c>
+      <c r="I46" s="2">
+        <f>AVERAGE(D46:D56)</f>
+        <v>0.94069090909090913</v>
+      </c>
+      <c r="J46" s="2">
+        <f>AVERAGE(E46:E56)</f>
+        <v>0.94395454545454538</v>
+      </c>
+      <c r="K46" s="2">
+        <f>MAX(C46:C56)</f>
+        <v>0.95894000000000001</v>
+      </c>
+      <c r="L46" s="2">
+        <f>MAX(D46:D56)</f>
+        <v>0.95020000000000004</v>
+      </c>
+      <c r="M46" s="2">
+        <f>MAX(E46:E56)</f>
+        <v>0.94810000000000005</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47">
         <v>20</v>
       </c>
@@ -1290,8 +1926,16 @@
       <c r="E47" s="2">
         <v>0.94030000000000002</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5359999999999929E-2</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="1"/>
+        <v>5.9999999999993392E-4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48">
         <v>20</v>
       </c>
@@ -1307,8 +1951,16 @@
       <c r="E48" s="2">
         <v>0.93989999999999996</v>
       </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5240000000000031E-2</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.6999999999999256E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49">
         <v>20</v>
       </c>
@@ -1324,8 +1976,16 @@
       <c r="E49" s="2">
         <v>0.94199999999999995</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="2">
+        <f t="shared" si="0"/>
+        <v>9.160000000000057E-3</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.0000000000000027E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50">
         <v>20</v>
       </c>
@@ -1341,8 +2001,16 @@
       <c r="E50" s="2">
         <v>0.94389999999999996</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2380000000000058E-2</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="1"/>
+        <v>-6.8999999999999062E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>20</v>
       </c>
@@ -1358,8 +2026,16 @@
       <c r="E51" s="2">
         <v>0.94120000000000004</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0079999999999978E-2</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="1"/>
+        <v>1.3999999999999568E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>20</v>
       </c>
@@ -1375,8 +2051,16 @@
       <c r="E52" s="2">
         <v>0.94179999999999997</v>
       </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="2">
+        <f t="shared" si="0"/>
+        <v>9.5399999999999929E-3</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="1"/>
+        <v>-8.69999999999993E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53">
         <v>20</v>
       </c>
@@ -1392,8 +2076,16 @@
       <c r="E53" s="2">
         <v>0.94810000000000005</v>
       </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0839999999999961E-2</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999908E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54">
         <v>20</v>
       </c>
@@ -1409,8 +2101,16 @@
       <c r="E54" s="2">
         <v>0.94640000000000002</v>
       </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1699999999999933E-2</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="1"/>
+        <v>-3.2999999999999696E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55">
         <v>20</v>
       </c>
@@ -1426,8 +2126,16 @@
       <c r="E55" s="2">
         <v>0.94540000000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999954E-2</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.9000000000000128E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56">
         <v>20</v>
       </c>
@@ -1442,6 +2150,14 @@
       </c>
       <c r="E56" s="2">
         <v>0.94699999999999995</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0980000000000101E-2</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="1"/>
+        <v>-5.0000000000000044E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>